<commit_message>
add fao to total luc differences
</commit_message>
<xml_diff>
--- a/results/standard/UNEP-EGR-2024-total-luc-differences.xlsx
+++ b/results/standard/UNEP-EGR-2024-total-luc-differences.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -51,22 +51,25 @@
     <t xml:space="preserve">units</t>
   </si>
   <si>
-    <t xml:space="preserve">BLUE</t>
+    <t xml:space="preserve">Bookkeeping | BLUE</t>
   </si>
   <si>
     <t xml:space="preserve">GtCO2/year</t>
   </si>
   <si>
-    <t xml:space="preserve">H&amp;N</t>
+    <t xml:space="preserve">Bookkeeping | H&amp;N</t>
   </si>
   <si>
-    <t xml:space="preserve">OSCAR</t>
+    <t xml:space="preserve">Bookkeeping | OSCAR</t>
   </si>
   <si>
-    <t xml:space="preserve">Bookkeeping average</t>
+    <t xml:space="preserve">Bookkeeping | average</t>
   </si>
   <si>
     <t xml:space="preserve">Inventories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAO</t>
   </si>
 </sst>
 </file>
@@ -2748,6 +2751,468 @@
         <v>13</v>
       </c>
     </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>1990</v>
+      </c>
+      <c r="B167" t="s">
+        <v>18</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1.7635435932</v>
+      </c>
+      <c r="D167" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>1991</v>
+      </c>
+      <c r="B168" t="s">
+        <v>18</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1.7635435932</v>
+      </c>
+      <c r="D168" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>1992</v>
+      </c>
+      <c r="B169" t="s">
+        <v>18</v>
+      </c>
+      <c r="C169" t="n">
+        <v>1.7635435931</v>
+      </c>
+      <c r="D169" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>1993</v>
+      </c>
+      <c r="B170" t="s">
+        <v>18</v>
+      </c>
+      <c r="C170" t="n">
+        <v>1.7639772221</v>
+      </c>
+      <c r="D170" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>1994</v>
+      </c>
+      <c r="B171" t="s">
+        <v>18</v>
+      </c>
+      <c r="C171" t="n">
+        <v>1.7636441844</v>
+      </c>
+      <c r="D171" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>1995</v>
+      </c>
+      <c r="B172" t="s">
+        <v>18</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1.7692517676</v>
+      </c>
+      <c r="D172" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>1996</v>
+      </c>
+      <c r="B173" t="s">
+        <v>18</v>
+      </c>
+      <c r="C173" t="n">
+        <v>1.6361572212</v>
+      </c>
+      <c r="D173" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B174" t="s">
+        <v>18</v>
+      </c>
+      <c r="C174" t="n">
+        <v>2.3259997112</v>
+      </c>
+      <c r="D174" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>1998</v>
+      </c>
+      <c r="B175" t="s">
+        <v>18</v>
+      </c>
+      <c r="C175" t="n">
+        <v>1.7700120542</v>
+      </c>
+      <c r="D175" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>1999</v>
+      </c>
+      <c r="B176" t="s">
+        <v>18</v>
+      </c>
+      <c r="C176" t="n">
+        <v>1.6736788596</v>
+      </c>
+      <c r="D176" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B177" t="s">
+        <v>18</v>
+      </c>
+      <c r="C177" t="n">
+        <v>1.6215367559</v>
+      </c>
+      <c r="D177" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B178" t="s">
+        <v>18</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1.3444369577</v>
+      </c>
+      <c r="D178" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B179" t="s">
+        <v>18</v>
+      </c>
+      <c r="C179" t="n">
+        <v>1.7201421788</v>
+      </c>
+      <c r="D179" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B180" t="s">
+        <v>18</v>
+      </c>
+      <c r="C180" t="n">
+        <v>1.4476078186</v>
+      </c>
+      <c r="D180" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B181" t="s">
+        <v>18</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1.7178166743</v>
+      </c>
+      <c r="D181" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B182" t="s">
+        <v>18</v>
+      </c>
+      <c r="C182" t="n">
+        <v>1.5112234373</v>
+      </c>
+      <c r="D182" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B183" t="s">
+        <v>18</v>
+      </c>
+      <c r="C183" t="n">
+        <v>1.8068813722</v>
+      </c>
+      <c r="D183" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B184" t="s">
+        <v>18</v>
+      </c>
+      <c r="C184" t="n">
+        <v>1.3808307486</v>
+      </c>
+      <c r="D184" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B185" t="s">
+        <v>18</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1.3687807169</v>
+      </c>
+      <c r="D185" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B186" t="s">
+        <v>18</v>
+      </c>
+      <c r="C186" t="n">
+        <v>1.6726327904</v>
+      </c>
+      <c r="D186" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B187" t="s">
+        <v>18</v>
+      </c>
+      <c r="C187" t="n">
+        <v>1.3818374722</v>
+      </c>
+      <c r="D187" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B188" t="s">
+        <v>18</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0.3066388384</v>
+      </c>
+      <c r="D188" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B189" t="s">
+        <v>18</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0.3161867504</v>
+      </c>
+      <c r="D189" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B190" t="s">
+        <v>18</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0.3019906273</v>
+      </c>
+      <c r="D190" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B191" t="s">
+        <v>18</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0.5654136678</v>
+      </c>
+      <c r="D191" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B192" t="s">
+        <v>18</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0.5815682263</v>
+      </c>
+      <c r="D192" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B193" t="s">
+        <v>18</v>
+      </c>
+      <c r="C193" t="n">
+        <v>1.1828981771</v>
+      </c>
+      <c r="D193" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B194" t="s">
+        <v>18</v>
+      </c>
+      <c r="C194" t="n">
+        <v>1.1479663139</v>
+      </c>
+      <c r="D194" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B195" t="s">
+        <v>18</v>
+      </c>
+      <c r="C195" t="n">
+        <v>1.2958760425</v>
+      </c>
+      <c r="D195" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B196" t="s">
+        <v>18</v>
+      </c>
+      <c r="C196" t="n">
+        <v>1.4706543365</v>
+      </c>
+      <c r="D196" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B197" t="s">
+        <v>18</v>
+      </c>
+      <c r="C197" t="n">
+        <v>1.1731730705</v>
+      </c>
+      <c r="D197" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B198" t="s">
+        <v>18</v>
+      </c>
+      <c r="C198" t="n">
+        <v>1.1535669849</v>
+      </c>
+      <c r="D198" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B199" t="s">
+        <v>18</v>
+      </c>
+      <c r="C199" t="n">
+        <v>1.145102449</v>
+      </c>
+      <c r="D199" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tweaks to LUC figure
</commit_message>
<xml_diff>
--- a/results/standard/UNEP-EGR-2024-total-luc-differences.xlsx
+++ b/results/standard/UNEP-EGR-2024-total-luc-differences.xlsx
@@ -51,19 +51,19 @@
     <t xml:space="preserve">units</t>
   </si>
   <si>
-    <t xml:space="preserve">Bookkeeping | BLUE</t>
+    <t xml:space="preserve">BLUE</t>
   </si>
   <si>
     <t xml:space="preserve">GtCO2/year</t>
   </si>
   <si>
-    <t xml:space="preserve">Bookkeeping | H&amp;N</t>
+    <t xml:space="preserve">H&amp;N</t>
   </si>
   <si>
-    <t xml:space="preserve">Bookkeeping | OSCAR</t>
+    <t xml:space="preserve">OSCAR</t>
   </si>
   <si>
-    <t xml:space="preserve">Bookkeeping | average</t>
+    <t xml:space="preserve">Bookkeeping average</t>
   </si>
   <si>
     <t xml:space="preserve">Inventories</t>

</xml_diff>

<commit_message>
new figure per capita vs change
</commit_message>
<xml_diff>
--- a/results/standard/UNEP-EGR-2024-total-luc-differences.xlsx
+++ b/results/standard/UNEP-EGR-2024-total-luc-differences.xlsx
@@ -66,10 +66,10 @@
     <t xml:space="preserve">Bookkeeping average</t>
   </si>
   <si>
-    <t xml:space="preserve">Inventories</t>
+    <t xml:space="preserve">Grassi NGHGI (inventories)</t>
   </si>
   <si>
-    <t xml:space="preserve">FAO</t>
+    <t xml:space="preserve">FAOSTAT</t>
   </si>
 </sst>
 </file>

</xml_diff>